<commit_message>
Ajout de quelques tests
</commit_message>
<xml_diff>
--- a/Test/test.xlsx
+++ b/Test/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1746B711-D6A5-437B-AB4F-A93A8719FA6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8144A841-CE29-4E31-B80F-A999B349939F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALIMENTATION" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="66">
   <si>
     <t>N°</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Vitesse d'interruption en mode FALLING</t>
   </si>
   <si>
-    <t>Lecture en boucle des entrées analogiques</t>
-  </si>
-  <si>
     <t>Affichage sur le port série de la tension des entrées analogiques.</t>
   </si>
   <si>
@@ -167,43 +164,67 @@
     <t>Commande d'un moteur CC</t>
   </si>
   <si>
-    <t>Le moteur tourne</t>
-  </si>
-  <si>
     <t>MP23017,  alimentation de table en 12V, programme "2.ino"</t>
   </si>
   <si>
-    <t>alimentation de table en 12V, programme "1.ino"</t>
-  </si>
-  <si>
     <t>La communications fonctionne, les niveaux de tensions sont bons, la fréquence est correct</t>
   </si>
   <si>
-    <t>Communication en I2C avec un module slave avec des fils court (&lt;50cm)</t>
-  </si>
-  <si>
     <t>MP23017,  alimentation de table en 12V, programme "3.ino"</t>
   </si>
   <si>
-    <t>Communication en I2C avec un module slave avec des fils long (&gt;1m)</t>
-  </si>
-  <si>
-    <t>Communication en SPI avec un module slave avec des fils court (&lt;50cm)</t>
-  </si>
-  <si>
-    <t>Communication en SPI avec un module slave avec des fils long (&gt;1m)</t>
-  </si>
-  <si>
-    <t>Communication en RS232 avec un module avec des fils court (&lt;50cm)</t>
-  </si>
-  <si>
-    <t>Communication en RS232 avec un module avec des fils long (&gt;1m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> alimentation de table en 12V, programme "1.ino"</t>
-  </si>
-  <si>
-    <t>Communication avec MySensor en nrf24 sur une courte distance</t>
+    <t>Les données s'échangent bien</t>
+  </si>
+  <si>
+    <t>alimentation de table en 12V, optocoupleur (ACPL-247-500E) avec résistance de pull-up de 1k et LED rouge / transistor NPN (MMPQ2222A) avec résistance sur base de 510, programme "1.ino"</t>
+  </si>
+  <si>
+    <t>Le moteur tourne correctement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alimentation de table en 12V, nrf52832 de I-SYST sur la UtiliPi v2.3, programme "1.ino"</t>
+  </si>
+  <si>
+    <t>Communication avec MySensor en nrf24 sur une courte distance (&lt;1m) et mesure de la perte de pacquet s'il y en a</t>
+  </si>
+  <si>
+    <t>RSSI ? Perte de pacquet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alimentation de table en 5V, nrf52832 de EBYTE sur le PCB de openhardware et avec une antenne, programme "1.ino"</t>
+  </si>
+  <si>
+    <t>Communication avec MySensor en nrf24 sur une longue distance (&gt;20m) et mesure de la perte de pacquet s'il y en a.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication avec MySensor en nrf24 sur une longue distance (&gt;20m) et en milieu industriel. Mesure de la perte de pacquet s'il y en a. </t>
+  </si>
+  <si>
+    <t>Communication en I2C avec un module slave avec des fils court (&lt;50cm) et à la fréquence max (400KHz)</t>
+  </si>
+  <si>
+    <t>Communication en I2C avec un module slave avec des fils long (&gt;2m) et à la fréquence max (400KHz)</t>
+  </si>
+  <si>
+    <t>Communication en SPI avec un module slave avec des fils court (&lt;50cm) et à la fréquence max (8MHz)</t>
+  </si>
+  <si>
+    <t>Communication en SPI avec un module slave avec des fils long (&gt;2m) et à la fréquence max (8MHz)</t>
+  </si>
+  <si>
+    <t>Communication en RS232 avec un module avec des fils court (&lt;50cm) et à la fréquence max (?)</t>
+  </si>
+  <si>
+    <t>Communication en RS232 avec un module avec des fils long (&gt;2m) et à la fréquence max (?)</t>
+  </si>
+  <si>
+    <t>alimentation de table en 12V, MCP3208, programme "1.ino"</t>
+  </si>
+  <si>
+    <t>Lecture en boucle des entrées analogiques en tension (0 ~ 10V)</t>
+  </si>
+  <si>
+    <t>Lecture en boucle des entrées analogiques en courant (4 ~ 20mA)</t>
   </si>
 </sst>
 </file>
@@ -266,27 +287,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -985,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,50 +1148,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1208,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F8F217-B8AA-4802-BCB3-0C3F86212780}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,7 +1343,9 @@
         <v>31</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1358,7 +1361,9 @@
         <v>31</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1376,50 +1381,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E5">
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1438,7 +1443,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,30 +1479,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
+      <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1541,18 +1550,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1571,7 +1580,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,65 +1611,65 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -1724,7 +1733,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,13 +1769,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -1775,13 +1784,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -1790,13 +1799,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
@@ -1806,13 +1815,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
@@ -1822,13 +1831,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
@@ -1838,13 +1847,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -1878,10 +1887,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1897,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36E4726-2BAD-4758-A1D3-4480B44D07F9}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,66 +1940,119 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="F7" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1999,8 +2061,23 @@
       <c r="D9" s="2"/>
       <c r="F9" s="2"/>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E4">
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3 E5:E7">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
@@ -2008,7 +2085,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
@@ -2017,7 +2094,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{297854E0-8F18-497D-88A0-0E906F960EBE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{297854E0-8F18-497D-88A0-0E906F960EBE}">
       <formula1>"OK,KO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Ajout de la version MCP23S17 SPI à la place du MCP23017 I2C
</commit_message>
<xml_diff>
--- a/Test/test.xlsx
+++ b/Test/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518E25FA-8FA3-4D9B-8148-EAED63811D05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812ADB39-31C8-4F59-B586-6F03B9C3254D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALIMENTATION" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="88">
   <si>
     <t>N°</t>
   </si>
@@ -73,24 +73,12 @@
     <t>Alimentation de table Velleman, module buck d'aliexpress basé sur le MP2307, régulateur 3V3 (698-9044), programme "3.ino"</t>
   </si>
   <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "1.ino"</t>
-  </si>
-  <si>
     <t>Alimentation de table Velleman, module buck d'aliexpress basé sur le MP2307, régulateur 3V3 (698-9044), programme "4.ino"</t>
   </si>
   <si>
     <t>Alimentation de table en 24V: mesure de consomation sur l'alimentation de table, mesure de consomation après le module buck. Mesure de consommation des TRANSISTORS à vide mais fermé.</t>
   </si>
   <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "2.ino"</t>
-  </si>
-  <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "3.ino"</t>
-  </si>
-  <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "4.ino"</t>
-  </si>
-  <si>
     <t>Vitesse de lecture avec digitalRead</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
   </si>
   <si>
     <t>Fréquence max :</t>
-  </si>
-  <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "5.ino", binaire au choix dans la stm32 nucleo</t>
   </si>
   <si>
     <t>Recevoir une PWM avec la fréquence la plus grande possible sur A0 depuis une STM32 nucleo. On sait si l'interruption est bien gérée en regardant le signal INTA à l'oscilloscope.</t>
@@ -126,12 +111,6 @@
   </si>
   <si>
     <t>Vitesse d'interruption en mode CHANGE</t>
-  </si>
-  <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "6.ino", binaire au choix dans la stm32 nucleo</t>
-  </si>
-  <si>
-    <t>MP23017, bibliothèque adafruit, alimentation de table en 12V, programme "7.ino", binaire au choix dans la stm32 nucleo</t>
   </si>
   <si>
     <t>Vitesse d'interruption en mode RISING</t>
@@ -253,6 +232,73 @@
   <si>
     <t>Consomation sur l'alimentation de table : 23mA
 Consomation après le module buck : 18,4 mA</t>
+  </si>
+  <si>
+    <t>Fréquence max : +60KHz
+Période min pour lire une entrée et faire baisser le flag d'interruption : 9,7µs</t>
+  </si>
+  <si>
+    <t>Recevoir une PWM avec la fréquence la plus grande possible sur A7 depuis une STM32 nucleo. On sait si l'interruption est bien gérée en regardant le signal INTA à l'oscilloscope.</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "8.ino"</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "9.ino"</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "10.ino"</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "11.ino"</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "1.ino"</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "2.ino"</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "3.ino"</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "4.ino"</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "5.ino", binaire au choix dans la stm32 nucleo</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "6.ino", binaire au choix dans la stm32 nucleo</t>
+  </si>
+  <si>
+    <t>MP23017, bibliothèque adafruit, alimentation de table en 24V, programme "7.ino", binaire au choix dans la stm32 nucleo</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "12.ino", binaire au choix dans la stm32 nucleo</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "13.ino", binaire au choix dans la stm32 nucleo</t>
+  </si>
+  <si>
+    <t>MP23S17, bibliothèque Adafruit modifié, alimentation de table en 24V, programme "14.ino", binaire au choix dans la stm32 nucleo</t>
+  </si>
+  <si>
+    <t>Pour 10V et une résistance de 100ohm, on obtiens un courant de 80mA au lieu de 100mA</t>
+  </si>
+  <si>
+    <t>Fréquence max : 24,1KHz (lecture du latch et ensuite écriture --&gt; 2 opérations sur le bus SPI)</t>
+  </si>
+  <si>
+    <t>Fréquence max : 30,3KHz (une seule écriture de registre --&gt; 1 seule opération sur le bus SPI)</t>
+  </si>
+  <si>
+    <t>Commande d'un relai en 24V</t>
+  </si>
+  <si>
+    <t>Le relai fait "click" et fait le contact</t>
+  </si>
+  <si>
+    <t>ça fait "click"</t>
   </si>
 </sst>
 </file>
@@ -294,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,11 +360,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -997,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,16 +1206,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1063,10 +1232,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1083,10 +1252,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1103,10 +1272,10 @@
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1132,19 +1301,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,50 +1339,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1229,17 +1398,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F8F217-B8AA-4802-BCB3-0C3F86212780}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1268,16 +1437,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1285,16 +1455,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1302,17 +1473,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1320,17 +1491,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1338,17 +1509,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1356,17 +1529,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1374,84 +1547,250 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E5">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="23" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="24" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="21" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="22" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E12">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8" xr:uid="{FB21C624-1F55-4C93-AD3E-EEA4B917F170}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{FB21C624-1F55-4C93-AD3E-EEA4B917F170}">
       <formula1>"OK,KO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1465,14 +1804,14 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1489,7 +1828,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1501,13 +1840,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -1516,15 +1855,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>30</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,7 +1870,6 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,18 +1909,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1601,15 +1938,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03CC262-7BB2-4EFB-AEC5-A80318CCC8BE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1626,7 +1963,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1638,30 +1975,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>33</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1669,15 +2010,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>33</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1685,22 +2025,35 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="F6" s="4"/>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1724,24 +2077,24 @@
       <c r="F9" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E4">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+  <conditionalFormatting sqref="E3:E6">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{F5DAB4E1-D6D6-4F5E-B2BD-4F419AF70DDA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{F5DAB4E1-D6D6-4F5E-B2BD-4F419AF70DDA}">
       <formula1>"OK,KO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1755,14 +2108,14 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1779,7 +2132,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1791,14 +2144,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E2" s="5"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1806,14 +2160,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1821,15 +2176,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>38</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1837,15 +2191,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>38</v>
+      </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1853,15 +2206,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>38</v>
+      </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1869,13 +2221,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -1909,10 +2261,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1931,14 +2283,14 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1955,7 +2307,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1967,16 +2319,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E2" s="5"/>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1984,17 +2337,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>40</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2002,17 +2354,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>40</v>
+      </c>
       <c r="F4" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2020,17 +2371,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>40</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2038,17 +2388,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>40</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2056,17 +2405,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>40</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2092,26 +2440,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3 E5:E7">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>